<commit_message>
Improving application UI code
</commit_message>
<xml_diff>
--- a/reports/asin_report.xlsx
+++ b/reports/asin_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,12 +508,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>UT-X84W-ZTPT</t>
+          <t>NG-IWXD-5PE7</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Majestic Pure Moroccan Argan Oil for Hair, Face, Nails, Beard &amp; Cuticles - for Men and Women - Pure &amp; Natural, 4 fl. oz.</t>
+          <t>Majestic Pure Bulgarian Lavender Essential Oil, 100% Pure and Natural with Therapeutic Grade, Premium Quality Bulgarian Lavender Oil, 1 fl. oz.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -523,26 +523,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>B00QVR0O6Q</t>
+          <t>B01FZRK3WW</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3581</v>
+        <v>354</v>
       </c>
       <c r="G2" t="n">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="H2" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>110,172</t>
+          <t>63,169</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1,048</t>
+          <t>366</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -565,12 +565,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CelluliteOil8oz</t>
+          <t>Acnea3ScarWashCleanser</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Majestic Pure Natural Cellulite Massage Oil, Unique Blend of Massage Essential Oils - Improves Skin Firmness, More Effective Than Cellulite Cream, 8 fl oz</t>
+          <t>MAJESTIC PURE Acnea3 Scar Acne Wash Foaming Facial Cleanser - Soothes Blemishes and Clears Pores, Made with Pure Peppermint and Tea Tree Essential Oils - for All Skin Types, 4 fl oz</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -580,39 +580,37 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>B07HFFMY2X</t>
+          <t>B07VXK2RX4</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>973</v>
-      </c>
-      <c r="G3" t="n">
-        <v>8</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>23,283</t>
+          <t>153,219</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>5,998</t>
-        </is>
-      </c>
+          <t>1,592</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Lose Q &amp; A, Sub.Cat2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -622,12 +620,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NG-IWXD-5PE7</t>
+          <t>6L-S5IM-ZW9C</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Majestic Pure Bulgarian Lavender Essential Oil, 100% Pure and Natural with Therapeutic Grade, Premium Quality Bulgarian Lavender Oil, 1 fl. oz.</t>
+          <t>Majestic Pure Fractionated Coconut Oil, For Aromatherapy Relaxing Massage, Carrier Oil for Diluting Essential Oils, Hair &amp; Skin Care Benefits, Moisturizer &amp; Softener - 16 Ounces (Packaging May Vary)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -637,26 +635,26 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>B01FZRK3WW</t>
+          <t>B00PMR3QF2</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>352</v>
+        <v>19164</v>
       </c>
       <c r="G4" t="n">
-        <v>25</v>
+        <v>394</v>
       </c>
       <c r="H4" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>79,767</t>
+          <t>583</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>492</t>
+          <t>14</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -679,12 +677,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Acnea3ScarWashCleanser</t>
+          <t>NewPeppermintOil</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MAJESTIC PURE Acnea3 Scar Acne Wash Foaming Facial Cleanser - Soothes Blemishes and Clears Pores, Made with Pure Peppermint and Tea Tree Essential Oils - for All Skin Types, 4 fl oz</t>
+          <t>Majestic Pure Peppermint Essential Oil, Pure and Natural, Therapeutic Grade Peppermint Oil, 4 fl. oz.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -694,24 +692,26 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>B07VXK2RX4</t>
+          <t>B00PV15BPW</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>210</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>12842</v>
+      </c>
+      <c r="G5" t="n">
+        <v>193</v>
+      </c>
       <c r="H5" t="n">
-        <v>4.1</v>
+        <v>4.7</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>112,165</t>
+          <t>3,519</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1,240</t>
+          <t>14</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -722,7 +722,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Lose Q &amp; A, Sub.Cat2</t>
+          <t>Lose Sub.Cat2</t>
         </is>
       </c>
     </row>
@@ -734,12 +734,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6L-S5IM-ZW9C</t>
+          <t>BX-N0NF-ETC9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Majestic Pure Fractionated Coconut Oil, For Aromatherapy Relaxing Massage, Carrier Oil for Diluting Essential Oils, Hair &amp; Skin Care Benefits, Moisturizer &amp; Softener - 16 Ounces (Packaging May Vary)</t>
+          <t>MAJESTIC PURE Indian Healing Clay Powder, Deep Pore Cleansing Facial, Body and Hair Mask, Natural Sodium Bentonite Clay, 16oz</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -749,26 +749,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>B00PMR3QF2</t>
+          <t>B00Q96XGUU</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>19144</v>
+        <v>1785</v>
       </c>
       <c r="G6" t="n">
-        <v>394</v>
+        <v>109</v>
       </c>
       <c r="H6" t="n">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>825</t>
+          <t>122,474</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>2,391</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -791,12 +791,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NewPeppermintOil</t>
+          <t>NewLemonOil</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Majestic Pure Peppermint Essential Oil, Pure and Natural, Therapeutic Grade Peppermint Oil, 4 fl. oz.</t>
+          <t>Majestic Pure Lemon Oil, Therapeutic Grade, Premium Quality Lemon Oil, 4 Ounces</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -806,26 +806,26 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>B00PV15BPW</t>
+          <t>B00QR6SS6O</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>12819</v>
+        <v>6769</v>
       </c>
       <c r="G7" t="n">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="H7" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3,834</t>
+          <t>5,597</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>26</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -848,12 +848,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BX-N0NF-ETC9</t>
+          <t>AJ-CD9K-SAOC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MAJESTIC PURE Indian Healing Clay Powder, Deep Pore Cleansing Facial, Body and Hair Mask, Natural Sodium Bentonite Clay, 16oz</t>
+          <t>Majestic Pure Rosehip Oil for Face, Nails, Hair and Skin, Pure &amp; Natural, Cold Pressed Premium Rose Hip Seed Oil, 4 oz</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -863,26 +863,26 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>B00Q96XGUU</t>
+          <t>B00QR7FTLU</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1783</v>
+        <v>4599</v>
       </c>
       <c r="G8" t="n">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="H8" t="n">
-        <v>4.3</v>
+        <v>4.6</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>95,731</t>
+          <t>14,832</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1,846</t>
+          <t>145</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -905,12 +905,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NewLemonOil</t>
+          <t>UT-X84W-ZTPT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Majestic Pure Lemon Oil, Therapeutic Grade, Premium Quality Lemon Oil, 4 Ounces</t>
+          <t>Majestic Pure Moroccan Argan Oil for Hair, Face, Nails, Beard &amp; Cuticles - for Men and Women - Pure &amp; Natural, 4 fl. oz.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -920,26 +920,26 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>B00QR6SS6O</t>
+          <t>B00QVR0O6Q</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>6760</v>
+        <v>3580</v>
       </c>
       <c r="G9" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H9" t="n">
         <v>4.6</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4,655</t>
+          <t>91,531</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>868</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -962,12 +962,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AJ-CD9K-SAOC</t>
+          <t>JB-RO97-9L06</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Majestic Pure Rosehip Oil for Face, Nails, Hair and Skin, Pure &amp; Natural, Cold Pressed Premium Rose Hip Seed Oil, 4 oz</t>
+          <t>Majestic Pure Jojoba Oil for Hair and Skin, 4 fl. oz.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -977,26 +977,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>B00QR7FTLU</t>
+          <t>B00STVN68K</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>4594</v>
+        <v>859</v>
       </c>
       <c r="G10" t="n">
-        <v>121</v>
+        <v>38</v>
       </c>
       <c r="H10" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>12,530</t>
+          <t>53,541</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>504</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JB-RO97-9L06</t>
+          <t>MY-ETEY-F5KK</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Majestic Pure Jojoba Oil for Hair and Skin, 4 fl. oz.</t>
+          <t>Majestic Pure Lavender Oil, Natural, Therapeutic Grade, Premium Quality Blend of Lavender Essential Oil, 4 fl. Oz</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1034,26 +1034,26 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>B00STVN68K</t>
+          <t>B00TSTZQEY</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>859</v>
+        <v>15736</v>
       </c>
       <c r="G11" t="n">
-        <v>38</v>
+        <v>217</v>
       </c>
       <c r="H11" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>35,464</t>
+          <t>4,373</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>19</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1076,12 +1076,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MY-ETEY-F5KK</t>
+          <t>9D-BZC2-93AO</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Majestic Pure Lavender Oil, Natural, Therapeutic Grade, Premium Quality Blend of Lavender Essential Oil, 4 fl. Oz</t>
+          <t>MAJESTIC PURE Dead Sea Mud Mask - Natural Face and Skin Care for Women and Men - Best Black Facial Cleansing Clay for Blackhead, Whitehead, Acne and Pores - 8.8 fl. Oz</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1091,26 +1091,26 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>B00TSTZQEY</t>
+          <t>B00UREAGU8</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>15714</v>
+        <v>5614</v>
       </c>
       <c r="G12" t="n">
-        <v>217</v>
+        <v>126</v>
       </c>
       <c r="H12" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4,630</t>
+          <t>4,324</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>59</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1122,6 +1122,446 @@
       <c r="M12" t="inlineStr">
         <is>
           <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LV-XBR2-FJDV</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Majestic Pure Castor Oil, 100% Natural Wonder Oil with Numerous Hair, Scalp, Skin and Nails Benefits - Packaging May Vary- 16 fl oz</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>B00XE58NJ8</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>838</v>
+      </c>
+      <c r="G13" t="n">
+        <v>59</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>44,194</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>420</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>KO-M9OF-WEJA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Majestic Pure Hair Loss Shampoo, Offers Natural Ingredient Based Effective Solution, Add Volume and Strengthen Hair, Sulfate Free, 14 DHT Blockers, for Men &amp; Women - 16 fl Oz</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>B016RQ8PRU</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1654</v>
+      </c>
+      <c r="G14" t="n">
+        <v>90</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>27,836</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>48-62AK-XNDW</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Majestic Pure Black Pepper Essential Oil, Pure and Natural with Therapeutic Grade, Premium Quality Black Pepper Oil, 4 fl. oz.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>B0172AL2PM</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>178</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>106,561</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>652</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7W-UX75-3750</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Majestic Pure Clary Sage Oil, Premium Quality, 4 fl. oz.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>B01767OTVK</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>667</v>
+      </c>
+      <c r="G16" t="n">
+        <v>25</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>58,813</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>G9-CLOG-DZRL</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Majestic Pure Juniper Oil, Premium Quality, 4 fl. oz</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>B0176UQBJU</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>473</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Lose Category, Sub. Cat, Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>KO-I58S-WEWY</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Majestic Pure Myrrh Oil, Premium Quality, 4 fl Oz</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>B0176YOIEQ</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1019</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>41,122</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2H-DX31-4SOC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Majestic Pure Coconut Milk Body Scrub, Anti Cellulite &amp; Exfoliator, Natural Skin Care Formula Helps with Stretch Marks, Eczema, Acne and Varicose Veins, 12 Oz</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>B01BHQ69S2</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>810</v>
+      </c>
+      <c r="G19" t="n">
+        <v>18</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>29,576</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Lose Sub.Cat2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Majestic Pure</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>4J-YNLD-KLGK</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Majestic Pure Grapefruit Essential Oil, Pure and Natural, Therapeutic Grade Grapefruit Oil, 4 fl. oz.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>B01BKALLBU</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>945</v>
+      </c>
+      <c r="G20" t="n">
+        <v>22</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Lose Category, Sub. Cat, Sub.Cat2</t>
         </is>
       </c>
     </row>

</xml_diff>